<commit_message>
Add new data from Spring 2019
</commit_message>
<xml_diff>
--- a/data/Cam_BundlingDisclosureLobbyist.xlsx
+++ b/data/Cam_BundlingDisclosureLobbyist.xlsx
@@ -384,18 +384,18 @@
     </row>
     <row outlineLevel="0" r="2">
       <c r="A2" s="0">
-        <v>12</v>
+        <v>234</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Senator Gerald Ortiz y Pino</t>
+          <t>Carl Trujillo Committee</t>
         </is>
       </c>
       <c r="C2" s="0">
-        <v>162</v>
+        <v>2351</v>
       </c>
       <c r="D2" s="1">
-        <v>40721</v>
+        <v>41648.6997956366</v>
       </c>
       <c r="E2" s="0">
         <v>2</v>
@@ -403,18 +403,18 @@
     </row>
     <row outlineLevel="0" r="3">
       <c r="A3" s="0">
-        <v>15</v>
+        <v>235</v>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Committee to Elect Me</t>
+          <t>Jim Trujillo Committee</t>
         </is>
       </c>
       <c r="C3" s="0">
-        <v>142</v>
+        <v>2351</v>
       </c>
       <c r="D3" s="1">
-        <v>40743.4063919792</v>
+        <v>41648.7022064815</v>
       </c>
       <c r="E3" s="0">
         <v>2</v>
@@ -422,18 +422,18 @@
     </row>
     <row outlineLevel="0" r="4">
       <c r="A4" s="0">
-        <v>24</v>
+        <v>236</v>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Rep. Nate Gentry</t>
+          <t>Jacob Candelaria Committee</t>
         </is>
       </c>
       <c r="C4" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D4" s="1">
-        <v>40913</v>
+        <v>41648.7032034722</v>
       </c>
       <c r="E4" s="0">
         <v>2</v>
@@ -441,18 +441,18 @@
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="0">
-        <v>26</v>
+        <v>237</v>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Senator Phil Griego</t>
+          <t>Joseph Cervantes Committee</t>
         </is>
       </c>
       <c r="C5" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D5" s="1">
-        <v>40913.5927007292</v>
+        <v>41648.7039840278</v>
       </c>
       <c r="E5" s="0">
         <v>2</v>
@@ -460,18 +460,18 @@
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0">
-        <v>27</v>
+        <v>238</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Rep. Andy Nunez</t>
+          <t>Carlos Cisneros Committee</t>
         </is>
       </c>
       <c r="C6" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D6" s="1">
-        <v>40913.594815706</v>
+        <v>41648.7047381597</v>
       </c>
       <c r="E6" s="0">
         <v>2</v>
@@ -479,18 +479,18 @@
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="0">
-        <v>28</v>
+        <v>239</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Rep. David Doyle</t>
+          <t>Stuart Ingle Committee</t>
         </is>
       </c>
       <c r="C7" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D7" s="1">
-        <v>40913.5958933681</v>
+        <v>41648.7054517361</v>
       </c>
       <c r="E7" s="0">
         <v>2</v>
@@ -498,18 +498,18 @@
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0">
-        <v>29</v>
+        <v>240</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Rep. Larry Larranaga</t>
+          <t>Richard Martinez Committee</t>
         </is>
       </c>
       <c r="C8" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D8" s="1">
-        <v>40913.597806713</v>
+        <v>41648.7062680903</v>
       </c>
       <c r="E8" s="0">
         <v>2</v>
@@ -517,18 +517,18 @@
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0">
-        <v>30</v>
+        <v>241</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Senator Mark Boitano</t>
+          <t>Lisa Torraco Committee</t>
         </is>
       </c>
       <c r="C9" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D9" s="1">
-        <v>40913.5997401273</v>
+        <v>41648.70776875</v>
       </c>
       <c r="E9" s="0">
         <v>2</v>
@@ -536,18 +536,18 @@
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0">
-        <v>31</v>
+        <v>242</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Rep. Tom Taylor</t>
+          <t>Bill Payne Committee</t>
         </is>
       </c>
       <c r="C10" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D10" s="1">
-        <v>40913.6012371528</v>
+        <v>41648.7086337153</v>
       </c>
       <c r="E10" s="0">
         <v>2</v>
@@ -555,18 +555,18 @@
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0">
-        <v>32</v>
+        <v>243</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Rep. Joseph Cervantes</t>
+          <t>Gary King Committee</t>
         </is>
       </c>
       <c r="C11" s="0">
-        <v>849</v>
+        <v>2351</v>
       </c>
       <c r="D11" s="1">
-        <v>40913.6058154282</v>
+        <v>41648.7224611111</v>
       </c>
       <c r="E11" s="0">
         <v>2</v>
@@ -574,18 +574,18 @@
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="0">
-        <v>33</v>
+        <v>244</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Senator Mary K. Papen</t>
+          <t>Re-elect State Representative Sandra Jeff</t>
         </is>
       </c>
       <c r="C12" s="0">
-        <v>849</v>
+        <v>2401</v>
       </c>
       <c r="D12" s="1">
-        <v>40913</v>
+        <v>41653</v>
       </c>
       <c r="E12" s="0">
         <v>2</v>
@@ -593,18 +593,18 @@
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="0">
-        <v>34</v>
+        <v>245</v>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>Senator George Munoz</t>
+          <t>Munoz for Senate</t>
         </is>
       </c>
       <c r="C13" s="0">
-        <v>849</v>
+        <v>2401</v>
       </c>
       <c r="D13" s="1">
-        <v>40913.6074247685</v>
+        <v>41653</v>
       </c>
       <c r="E13" s="0">
         <v>2</v>
@@ -612,18 +612,18 @@
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="0">
-        <v>35</v>
+        <v>246</v>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>Senator Bill Payne</t>
+          <t>Michael Padilla</t>
         </is>
       </c>
       <c r="C14" s="0">
-        <v>849</v>
+        <v>2515</v>
       </c>
       <c r="D14" s="1">
-        <v>40913</v>
+        <v>41661</v>
       </c>
       <c r="E14" s="0">
         <v>2</v>
@@ -631,18 +631,18 @@
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="0">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>PAC-22</t>
+          <t>Emily Kane</t>
         </is>
       </c>
       <c r="C15" s="0">
-        <v>834</v>
+        <v>2515</v>
       </c>
       <c r="D15" s="1">
-        <v>40915</v>
+        <v>41661</v>
       </c>
       <c r="E15" s="0">
         <v>2</v>
@@ -650,18 +650,18 @@
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="0">
-        <v>38</v>
+        <v>248</v>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Multiple candidates</t>
+          <t>Lisa Torraco</t>
         </is>
       </c>
       <c r="C16" s="0">
-        <v>762</v>
+        <v>2515</v>
       </c>
       <c r="D16" s="1">
-        <v>40917</v>
+        <v>41661.6273397801</v>
       </c>
       <c r="E16" s="0">
         <v>2</v>
@@ -669,18 +669,18 @@
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="0">
-        <v>101</v>
+        <v>249</v>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>NM Senate Majority Leadership Fund</t>
+          <t>Mark Moores</t>
         </is>
       </c>
       <c r="C17" s="0">
-        <v>1030</v>
+        <v>2515</v>
       </c>
       <c r="D17" s="1">
-        <v>40921.4935462153</v>
+        <v>41661.6283504977</v>
       </c>
       <c r="E17" s="0">
         <v>2</v>
@@ -688,18 +688,18 @@
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="0">
-        <v>102</v>
+        <v>250</v>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>Comm to Elect Tom Taylor</t>
+          <t>Nate Gentry</t>
         </is>
       </c>
       <c r="C18" s="0">
-        <v>1030</v>
+        <v>2515</v>
       </c>
       <c r="D18" s="1">
-        <v>40921.5039724884</v>
+        <v>41661.6289706366</v>
       </c>
       <c r="E18" s="0">
         <v>2</v>
@@ -707,18 +707,18 @@
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="0">
-        <v>103</v>
+        <v>251</v>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>Governor Martinez PAC</t>
+          <t>Carl Trujillo</t>
         </is>
       </c>
       <c r="C19" s="0">
-        <v>1030</v>
+        <v>2515</v>
       </c>
       <c r="D19" s="1">
-        <v>40921.5472732639</v>
+        <v>41661.6298482639</v>
       </c>
       <c r="E19" s="0">
         <v>2</v>
@@ -726,18 +726,18 @@
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="0">
-        <v>105</v>
+        <v>252</v>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Susana Martinez for Governor</t>
+          <t>John Sapien</t>
         </is>
       </c>
       <c r="C20" s="0">
-        <v>1018</v>
+        <v>2515</v>
       </c>
       <c r="D20" s="1">
-        <v>40924</v>
+        <v>41661.6392118866</v>
       </c>
       <c r="E20" s="0">
         <v>2</v>
@@ -745,37 +745,37 @@
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="0">
-        <v>109</v>
+        <v>253</v>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>andy nunez</t>
+          <t>Phil Griego</t>
         </is>
       </c>
       <c r="C21" s="0">
-        <v>1198</v>
+        <v>2515</v>
       </c>
       <c r="D21" s="1">
-        <v>40963.3727584143</v>
+        <v>41661.6401135764</v>
       </c>
       <c r="E21" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="0">
-        <v>111</v>
+        <v>254</v>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>David Ulibarri</t>
+          <t>Pete Campos</t>
         </is>
       </c>
       <c r="C22" s="0">
-        <v>1048</v>
+        <v>2515</v>
       </c>
       <c r="D22" s="1">
-        <v>40969.453783831</v>
+        <v>41661.6407568287</v>
       </c>
       <c r="E22" s="0">
         <v>2</v>
@@ -783,18 +783,18 @@
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="0">
-        <v>112</v>
+        <v>255</v>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>Tom Taylor</t>
+          <t>Stephanie Garcia-Richard</t>
         </is>
       </c>
       <c r="C23" s="0">
-        <v>1048</v>
+        <v>2515</v>
       </c>
       <c r="D23" s="1">
-        <v>40969.4551866551</v>
+        <v>41661.6415364583</v>
       </c>
       <c r="E23" s="0">
         <v>2</v>
@@ -802,18 +802,18 @@
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="0">
-        <v>113</v>
+        <v>256</v>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Bill Sharer</t>
+          <t>Monica Youngblood</t>
         </is>
       </c>
       <c r="C24" s="0">
-        <v>1048</v>
+        <v>2515</v>
       </c>
       <c r="D24" s="1">
-        <v>40969.4562753125</v>
+        <v>41661.6422158912</v>
       </c>
       <c r="E24" s="0">
         <v>2</v>
@@ -821,18 +821,18 @@
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="0">
-        <v>115</v>
+        <v>266</v>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Debbie Rodella</t>
+          <t>Committee to elect Luciano Varela</t>
         </is>
       </c>
       <c r="C25" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D25" s="1">
-        <v>40969</v>
+        <v>41995.2755185185</v>
       </c>
       <c r="E25" s="0">
         <v>2</v>
@@ -840,18 +840,18 @@
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="0">
-        <v>116</v>
+        <v>267</v>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>Henry Saavedra</t>
+          <t>Committee to elect Rodney Montoya</t>
         </is>
       </c>
       <c r="C26" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D26" s="1">
-        <v>40969.4643073727</v>
+        <v>41995</v>
       </c>
       <c r="E26" s="0">
         <v>2</v>
@@ -859,18 +859,18 @@
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="0">
-        <v>117</v>
+        <v>268</v>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>Bill Payne</t>
+          <t>Committee to elect James Strickler</t>
         </is>
       </c>
       <c r="C27" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D27" s="1">
-        <v>40969.4652428588</v>
+        <v>41995</v>
       </c>
       <c r="E27" s="0">
         <v>2</v>
@@ -878,18 +878,18 @@
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="0">
-        <v>118</v>
+        <v>269</v>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>John Ryan</t>
+          <t>Committee to elect Paul Bandy</t>
         </is>
       </c>
       <c r="C28" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D28" s="1">
-        <v>40969.4659270023</v>
+        <v>41995</v>
       </c>
       <c r="E28" s="0">
         <v>2</v>
@@ -897,18 +897,18 @@
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="0">
-        <v>119</v>
+        <v>270</v>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>Steve Neville</t>
+          <t>Committee to elect Sharon Clahchischilliage</t>
         </is>
       </c>
       <c r="C29" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D29" s="1">
-        <v>40969.467762581</v>
+        <v>41995.2819042824</v>
       </c>
       <c r="E29" s="0">
         <v>2</v>
@@ -916,18 +916,18 @@
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="0">
-        <v>120</v>
+        <v>271</v>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>Richard Martinez</t>
+          <t>Committee to elect Kelly Fajardo</t>
         </is>
       </c>
       <c r="C30" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D30" s="1">
-        <v>40969.4687997338</v>
+        <v>41995</v>
       </c>
       <c r="E30" s="0">
         <v>2</v>
@@ -935,18 +935,18 @@
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="0">
-        <v>121</v>
+        <v>272</v>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>Stuart Ingle</t>
+          <t>Committee to elect Alonzo Baldonado</t>
         </is>
       </c>
       <c r="C31" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D31" s="1">
-        <v>40969.4695037847</v>
+        <v>41995</v>
       </c>
       <c r="E31" s="0">
         <v>2</v>
@@ -954,18 +954,18 @@
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="0">
-        <v>122</v>
+        <v>273</v>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>Clint Harden</t>
+          <t>Committee to elect Sarah Maestas-Barnes</t>
         </is>
       </c>
       <c r="C32" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D32" s="1">
-        <v>40969</v>
+        <v>41995</v>
       </c>
       <c r="E32" s="0">
         <v>2</v>
@@ -973,18 +973,18 @@
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="0">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>Carlos Cisneros</t>
+          <t>Committee to elect James Smith</t>
         </is>
       </c>
       <c r="C33" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D33" s="1">
-        <v>40969.4711525116</v>
+        <v>41995</v>
       </c>
       <c r="E33" s="0">
         <v>2</v>
@@ -992,18 +992,18 @@
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="0">
-        <v>124</v>
+        <v>275</v>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>Vernon Asbill</t>
+          <t>Committee to elect Paul Pacheco</t>
         </is>
       </c>
       <c r="C34" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D34" s="1">
-        <v>40969</v>
+        <v>41995</v>
       </c>
       <c r="E34" s="0">
         <v>2</v>
@@ -1011,18 +1011,18 @@
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="0">
-        <v>125</v>
+        <v>276</v>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>Rod Adair</t>
+          <t>Committee to elect Conrad James</t>
         </is>
       </c>
       <c r="C35" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D35" s="1">
-        <v>40969.4731597222</v>
+        <v>41995</v>
       </c>
       <c r="E35" s="0">
         <v>2</v>
@@ -1030,18 +1030,18 @@
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="0">
-        <v>126</v>
+        <v>277</v>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>Phil Griego</t>
+          <t>Committee to elect Lorenzo Larranaga</t>
         </is>
       </c>
       <c r="C36" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D36" s="1">
-        <v>40969.4739550926</v>
+        <v>41995</v>
       </c>
       <c r="E36" s="0">
         <v>2</v>
@@ -1049,18 +1049,18 @@
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="0">
-        <v>127</v>
+        <v>278</v>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>Susana Martinez</t>
+          <t>Committee to elect Jimmie Hall</t>
         </is>
       </c>
       <c r="C37" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D37" s="1">
-        <v>40969.4746129977</v>
+        <v>41995</v>
       </c>
       <c r="E37" s="0">
         <v>2</v>
@@ -1068,18 +1068,18 @@
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="0">
-        <v>129</v>
+        <v>279</v>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>Tim Lewis</t>
+          <t>Committee to elect Nate Gentry</t>
         </is>
       </c>
       <c r="C38" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D38" s="1">
-        <v>40969.5033022338</v>
+        <v>41995</v>
       </c>
       <c r="E38" s="0">
         <v>2</v>
@@ -1087,18 +1087,18 @@
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="0">
-        <v>130</v>
+        <v>280</v>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>Michael Sanchez</t>
+          <t>Committee to elect William Rehm</t>
         </is>
       </c>
       <c r="C39" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D39" s="1">
-        <v>40969</v>
+        <v>41995</v>
       </c>
       <c r="E39" s="0">
         <v>2</v>
@@ -1106,18 +1106,18 @@
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="0">
-        <v>131</v>
+        <v>281</v>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>Stuart Ingle</t>
+          <t>Committee to elect Dona Irwin</t>
         </is>
       </c>
       <c r="C40" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D40" s="1">
-        <v>40969.5283819792</v>
+        <v>41995</v>
       </c>
       <c r="E40" s="0">
         <v>2</v>
@@ -1125,18 +1125,18 @@
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="0">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>Bill Sharer</t>
+          <t>Committee to elect Andrew Nunez</t>
         </is>
       </c>
       <c r="C41" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D41" s="1">
-        <v>40969.5291003125</v>
+        <v>41995</v>
       </c>
       <c r="E41" s="0">
         <v>2</v>
@@ -1144,18 +1144,18 @@
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="0">
-        <v>133</v>
+        <v>283</v>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>Bill Payne</t>
+          <t>Committee to elect Terry Mcmillan</t>
         </is>
       </c>
       <c r="C42" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D42" s="1">
-        <v>40969.5297082986</v>
+        <v>41995</v>
       </c>
       <c r="E42" s="0">
         <v>2</v>
@@ -1163,18 +1163,18 @@
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="0">
-        <v>134</v>
+        <v>284</v>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>Steve Neville</t>
+          <t>Committee to elect Diane Hamilton</t>
         </is>
       </c>
       <c r="C43" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D43" s="1">
-        <v>40969.5303155903</v>
+        <v>41995</v>
       </c>
       <c r="E43" s="0">
         <v>2</v>
@@ -1182,18 +1182,18 @@
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="0">
-        <v>135</v>
+        <v>285</v>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>Phil Griego</t>
+          <t>Committee to elect Jane Powdrell-Culbert</t>
         </is>
       </c>
       <c r="C44" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D44" s="1">
-        <v>40969.5310568634</v>
+        <v>41995</v>
       </c>
       <c r="E44" s="0">
         <v>2</v>
@@ -1201,18 +1201,18 @@
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="0">
-        <v>136</v>
+        <v>286</v>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>David Ulibarri</t>
+          <t>Committee to elect Carl Trujillo</t>
         </is>
       </c>
       <c r="C45" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D45" s="1">
-        <v>40969.5316287037</v>
+        <v>41995</v>
       </c>
       <c r="E45" s="0">
         <v>2</v>
@@ -1220,18 +1220,18 @@
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="0">
-        <v>137</v>
+        <v>287</v>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>Richard Martinez</t>
+          <t>Committee to elect Don Tripp</t>
         </is>
       </c>
       <c r="C46" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D46" s="1">
-        <v>40969.5321478819</v>
+        <v>41995</v>
       </c>
       <c r="E46" s="0">
         <v>2</v>
@@ -1239,18 +1239,18 @@
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="0">
-        <v>138</v>
+        <v>288</v>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>George Munoz</t>
+          <t>Committee to elect Yvette Herrell</t>
         </is>
       </c>
       <c r="C47" s="0">
-        <v>1048</v>
+        <v>3012</v>
       </c>
       <c r="D47" s="1">
-        <v>40969.532846331</v>
+        <v>41995</v>
       </c>
       <c r="E47" s="0">
         <v>2</v>
@@ -1258,18 +1258,18 @@
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="0">
-        <v>139</v>
+        <v>289</v>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>Susana PAC</t>
+          <t>Committee to elect Ricky Little</t>
         </is>
       </c>
       <c r="C48" s="0">
-        <v>1270</v>
+        <v>3012</v>
       </c>
       <c r="D48" s="1">
-        <v>41022</v>
+        <v>41995</v>
       </c>
       <c r="E48" s="0">
         <v>2</v>
@@ -1277,56 +1277,56 @@
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="0">
-        <v>140</v>
+        <v>290</v>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Committee to elect Cathrynn Brown</t>
         </is>
       </c>
       <c r="C49" s="0">
-        <v>1271</v>
+        <v>3012</v>
       </c>
       <c r="D49" s="1">
-        <v>41022.364206794</v>
+        <v>41995</v>
       </c>
       <c r="E49" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="0">
-        <v>141</v>
+        <v>291</v>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>Committee to elect Jason Harper</t>
         </is>
       </c>
       <c r="C50" s="0">
-        <v>1271</v>
+        <v>3012</v>
       </c>
       <c r="D50" s="1">
-        <v>41022.3665546644</v>
+        <v>41995</v>
       </c>
       <c r="E50" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="0">
-        <v>142</v>
+        <v>292</v>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>Phil Griego Committee</t>
+          <t>Committee to elect Candy Ezzell</t>
         </is>
       </c>
       <c r="C51" s="0">
-        <v>1270</v>
+        <v>3012</v>
       </c>
       <c r="D51" s="1">
-        <v>41022.5227876968</v>
+        <v>41995</v>
       </c>
       <c r="E51" s="0">
         <v>2</v>
@@ -1334,37 +1334,37 @@
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="0">
-        <v>143</v>
+        <v>293</v>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Committee to elect Nora Espinoza</t>
         </is>
       </c>
       <c r="C52" s="0">
-        <v>1313</v>
+        <v>3012</v>
       </c>
       <c r="D52" s="1">
-        <v>41024.7078077894</v>
+        <v>41995</v>
       </c>
       <c r="E52" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="0">
-        <v>144</v>
+        <v>294</v>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>Legislature</t>
+          <t>Committee to elect Tim Lewis</t>
         </is>
       </c>
       <c r="C53" s="0">
-        <v>1367</v>
+        <v>3012</v>
       </c>
       <c r="D53" s="1">
-        <v>41026.4807114236</v>
+        <v>41995</v>
       </c>
       <c r="E53" s="0">
         <v>2</v>
@@ -1372,18 +1372,18 @@
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="0">
-        <v>156</v>
+        <v>295</v>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>John Smith Committee</t>
+          <t>Committee to elect David Gallegos</t>
         </is>
       </c>
       <c r="C54" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D54" s="1">
-        <v>41282</v>
+        <v>41995</v>
       </c>
       <c r="E54" s="0">
         <v>2</v>
@@ -1391,18 +1391,18 @@
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="0">
-        <v>157</v>
+        <v>296</v>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>Tom Taylor Committee</t>
+          <t>Committee to elect Larry Scott</t>
         </is>
       </c>
       <c r="C55" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D55" s="1">
-        <v>41282</v>
+        <v>41995</v>
       </c>
       <c r="E55" s="0">
         <v>2</v>
@@ -1410,18 +1410,18 @@
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="0">
-        <v>158</v>
+        <v>297</v>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>Carl Trujillo Committee</t>
+          <t>Committee to elect George Dodge</t>
         </is>
       </c>
       <c r="C56" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D56" s="1">
-        <v>41282.581194294</v>
+        <v>41995</v>
       </c>
       <c r="E56" s="0">
         <v>2</v>
@@ -1429,18 +1429,18 @@
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="0">
-        <v>159</v>
+        <v>298</v>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>Nancy Rodiguez Committee</t>
+          <t>Committee to elect James Madelena</t>
         </is>
       </c>
       <c r="C57" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D57" s="1">
-        <v>41282</v>
+        <v>41995</v>
       </c>
       <c r="E57" s="0">
         <v>2</v>
@@ -1448,18 +1448,18 @@
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="0">
-        <v>160</v>
+        <v>299</v>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
-          <t>Phil Griego Committee</t>
+          <t>Committee to elect Bob Wooley</t>
         </is>
       </c>
       <c r="C58" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D58" s="1">
-        <v>41282</v>
+        <v>41995</v>
       </c>
       <c r="E58" s="0">
         <v>2</v>
@@ -1467,18 +1467,18 @@
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="0">
-        <v>162</v>
+        <v>300</v>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
-          <t>Governor Susana Martinez</t>
+          <t>Committee to elect Dennis Roch</t>
         </is>
       </c>
       <c r="C59" s="0">
-        <v>1600</v>
+        <v>3012</v>
       </c>
       <c r="D59" s="1">
-        <v>41283</v>
+        <v>41995</v>
       </c>
       <c r="E59" s="0">
         <v>2</v>
@@ -1486,18 +1486,18 @@
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="0">
-        <v>163</v>
+        <v>301</v>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
-          <t>Paul Pacheco Committee</t>
+          <t>Committee to elect Monica Youngblood</t>
         </is>
       </c>
       <c r="C60" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D60" s="1">
-        <v>41283</v>
+        <v>41995</v>
       </c>
       <c r="E60" s="0">
         <v>2</v>
@@ -1505,18 +1505,18 @@
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="0">
-        <v>164</v>
+        <v>302</v>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>Tom Taylor Committee</t>
+          <t>Committee to elect Ken Martinez</t>
         </is>
       </c>
       <c r="C61" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D61" s="1">
-        <v>41283.4961366088</v>
+        <v>41995</v>
       </c>
       <c r="E61" s="0">
         <v>2</v>
@@ -1524,18 +1524,18 @@
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="0">
-        <v>165</v>
+        <v>303</v>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>Ken Martinez Committee</t>
+          <t>Committee to elect Vickie Perea</t>
         </is>
       </c>
       <c r="C62" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D62" s="1">
-        <v>41283.4972309028</v>
+        <v>41995</v>
       </c>
       <c r="E62" s="0">
         <v>2</v>
@@ -1543,18 +1543,18 @@
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="0">
-        <v>166</v>
+        <v>304</v>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>
-          <t>Michael Sanchez Committee</t>
+          <t>Committee to elect Geoff Rodgers</t>
         </is>
       </c>
       <c r="C63" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D63" s="1">
-        <v>41283.4980327546</v>
+        <v>41995</v>
       </c>
       <c r="E63" s="0">
         <v>2</v>
@@ -1562,18 +1562,18 @@
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="0">
-        <v>167</v>
+        <v>305</v>
       </c>
       <c r="B64" s="0" t="inlineStr">
         <is>
-          <t>Lee Alcon Committee</t>
+          <t>Committee to elect Betty Bishop</t>
         </is>
       </c>
       <c r="C64" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D64" s="1">
-        <v>41283</v>
+        <v>41995</v>
       </c>
       <c r="E64" s="0">
         <v>2</v>
@@ -1581,18 +1581,18 @@
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="0">
-        <v>168</v>
+        <v>306</v>
       </c>
       <c r="B65" s="0" t="inlineStr">
         <is>
-          <t>Lynda Lovejoy Committee</t>
+          <t>Committee to elect Johnny Luevano</t>
         </is>
       </c>
       <c r="C65" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D65" s="1">
-        <v>41283</v>
+        <v>41995</v>
       </c>
       <c r="E65" s="0">
         <v>2</v>
@@ -1600,18 +1600,18 @@
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="0">
-        <v>169</v>
+        <v>307</v>
       </c>
       <c r="B66" s="0" t="inlineStr">
         <is>
-          <t>Yvette Herrell  Committee</t>
+          <t>Committee to elect Sandra Jeff</t>
         </is>
       </c>
       <c r="C66" s="0">
-        <v>1614</v>
+        <v>3012</v>
       </c>
       <c r="D66" s="1">
-        <v>41283</v>
+        <v>41995</v>
       </c>
       <c r="E66" s="0">
         <v>2</v>
@@ -1619,18 +1619,18 @@
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="0">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="B67" s="0" t="inlineStr">
         <is>
-          <t>Larry Larranga Committee</t>
+          <t>Senator Gerald Ortiz y Pino</t>
         </is>
       </c>
       <c r="C67" s="0">
-        <v>1614</v>
+        <v>162</v>
       </c>
       <c r="D67" s="1">
-        <v>41283</v>
+        <v>40721</v>
       </c>
       <c r="E67" s="0">
         <v>2</v>
@@ -1638,18 +1638,18 @@
     </row>
     <row outlineLevel="0" r="68">
       <c r="A68" s="0">
-        <v>171</v>
+        <v>15</v>
       </c>
       <c r="B68" s="0" t="inlineStr">
         <is>
-          <t>House R Leadership Fund</t>
+          <t>Committee to Elect Me</t>
         </is>
       </c>
       <c r="C68" s="0">
-        <v>1614</v>
+        <v>142</v>
       </c>
       <c r="D68" s="1">
-        <v>41283</v>
+        <v>40743.4063919792</v>
       </c>
       <c r="E68" s="0">
         <v>2</v>
@@ -1657,18 +1657,18 @@
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="0">
-        <v>172</v>
+        <v>24</v>
       </c>
       <c r="B69" s="0" t="inlineStr">
         <is>
-          <t>ReElect Sen. Richard C. Martinez</t>
+          <t>Rep. Nate Gentry</t>
         </is>
       </c>
       <c r="C69" s="0">
-        <v>1702</v>
+        <v>849</v>
       </c>
       <c r="D69" s="1">
-        <v>41284.4519641551</v>
+        <v>40913</v>
       </c>
       <c r="E69" s="0">
         <v>2</v>
@@ -1676,18 +1676,18 @@
     </row>
     <row outlineLevel="0" r="70">
       <c r="A70" s="0">
-        <v>173</v>
+        <v>26</v>
       </c>
       <c r="B70" s="0" t="inlineStr">
         <is>
-          <t>Rep. Ray Begaye</t>
+          <t>Senator Phil Griego</t>
         </is>
       </c>
       <c r="C70" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D70" s="1">
-        <v>41289</v>
+        <v>40913.5927007292</v>
       </c>
       <c r="E70" s="0">
         <v>2</v>
@@ -1695,18 +1695,18 @@
     </row>
     <row outlineLevel="0" r="71">
       <c r="A71" s="0">
-        <v>174</v>
+        <v>27</v>
       </c>
       <c r="B71" s="0" t="inlineStr">
         <is>
-          <t>Sen. Tim Jennings</t>
+          <t>Rep. Andy Nunez</t>
         </is>
       </c>
       <c r="C71" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D71" s="1">
-        <v>41289.5752457523</v>
+        <v>40913.594815706</v>
       </c>
       <c r="E71" s="0">
         <v>2</v>
@@ -1714,18 +1714,18 @@
     </row>
     <row outlineLevel="0" r="72">
       <c r="A72" s="0">
-        <v>175</v>
+        <v>28</v>
       </c>
       <c r="B72" s="0" t="inlineStr">
         <is>
-          <t>Rep. Tim Lewis</t>
+          <t>Rep. David Doyle</t>
         </is>
       </c>
       <c r="C72" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D72" s="1">
-        <v>41289.576412581</v>
+        <v>40913.5958933681</v>
       </c>
       <c r="E72" s="0">
         <v>2</v>
@@ -1733,18 +1733,18 @@
     </row>
     <row outlineLevel="0" r="73">
       <c r="A73" s="0">
-        <v>176</v>
+        <v>29</v>
       </c>
       <c r="B73" s="0" t="inlineStr">
         <is>
-          <t>Rep. Nate Gentry</t>
+          <t>Rep. Larry Larranaga</t>
         </is>
       </c>
       <c r="C73" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D73" s="1">
-        <v>41289.5773395833</v>
+        <v>40913.597806713</v>
       </c>
       <c r="E73" s="0">
         <v>2</v>
@@ -1752,18 +1752,18 @@
     </row>
     <row outlineLevel="0" r="74">
       <c r="A74" s="0">
-        <v>177</v>
+        <v>30</v>
       </c>
       <c r="B74" s="0" t="inlineStr">
         <is>
-          <t>Rep. Alonzo Baldonado</t>
+          <t>Senator Mark Boitano</t>
         </is>
       </c>
       <c r="C74" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D74" s="1">
-        <v>41289.578472419</v>
+        <v>40913.5997401273</v>
       </c>
       <c r="E74" s="0">
         <v>2</v>
@@ -1771,18 +1771,18 @@
     </row>
     <row outlineLevel="0" r="75">
       <c r="A75" s="0">
-        <v>178</v>
+        <v>31</v>
       </c>
       <c r="B75" s="0" t="inlineStr">
         <is>
-          <t>Rep. Conrad James</t>
+          <t>Rep. Tom Taylor</t>
         </is>
       </c>
       <c r="C75" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D75" s="1">
-        <v>41289.5793075579</v>
+        <v>40913.6012371528</v>
       </c>
       <c r="E75" s="0">
         <v>2</v>
@@ -1790,18 +1790,18 @@
     </row>
     <row outlineLevel="0" r="76">
       <c r="A76" s="0">
-        <v>179</v>
+        <v>32</v>
       </c>
       <c r="B76" s="0" t="inlineStr">
         <is>
-          <t>Rep. Ed Sandoval</t>
+          <t>Rep. Joseph Cervantes</t>
         </is>
       </c>
       <c r="C76" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D76" s="1">
-        <v>41289.5827920486</v>
+        <v>40913.6058154282</v>
       </c>
       <c r="E76" s="0">
         <v>2</v>
@@ -1809,18 +1809,18 @@
     </row>
     <row outlineLevel="0" r="77">
       <c r="A77" s="0">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="B77" s="0" t="inlineStr">
         <is>
-          <t>Marci Blaze</t>
+          <t>Senator Mary K. Papen</t>
         </is>
       </c>
       <c r="C77" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D77" s="1">
-        <v>41289.5839465625</v>
+        <v>40913</v>
       </c>
       <c r="E77" s="0">
         <v>2</v>
@@ -1828,18 +1828,18 @@
     </row>
     <row outlineLevel="0" r="78">
       <c r="A78" s="0">
-        <v>181</v>
+        <v>34</v>
       </c>
       <c r="B78" s="0" t="inlineStr">
         <is>
-          <t>Clemente Sanchez</t>
+          <t>Senator George Munoz</t>
         </is>
       </c>
       <c r="C78" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D78" s="1">
-        <v>41289.5850884259</v>
+        <v>40913.6074247685</v>
       </c>
       <c r="E78" s="0">
         <v>2</v>
@@ -1847,18 +1847,18 @@
     </row>
     <row outlineLevel="0" r="79">
       <c r="A79" s="0">
-        <v>182</v>
+        <v>35</v>
       </c>
       <c r="B79" s="0" t="inlineStr">
         <is>
-          <t>Bill McCamley</t>
+          <t>Senator Bill Payne</t>
         </is>
       </c>
       <c r="C79" s="0">
-        <v>1793</v>
+        <v>849</v>
       </c>
       <c r="D79" s="1">
-        <v>41289.5863151273</v>
+        <v>40913</v>
       </c>
       <c r="E79" s="0">
         <v>2</v>
@@ -1866,18 +1866,18 @@
     </row>
     <row outlineLevel="0" r="80">
       <c r="A80" s="0">
-        <v>183</v>
+        <v>36</v>
       </c>
       <c r="B80" s="0" t="inlineStr">
         <is>
-          <t>Stephen Easley</t>
+          <t>PAC-22</t>
         </is>
       </c>
       <c r="C80" s="0">
-        <v>1793</v>
+        <v>834</v>
       </c>
       <c r="D80" s="1">
-        <v>41289.5879890046</v>
+        <v>40915</v>
       </c>
       <c r="E80" s="0">
         <v>2</v>
@@ -1885,18 +1885,18 @@
     </row>
     <row outlineLevel="0" r="81">
       <c r="A81" s="0">
-        <v>184</v>
+        <v>38</v>
       </c>
       <c r="B81" s="0" t="inlineStr">
         <is>
-          <t>Jeff Steinborn</t>
+          <t>Multiple candidates</t>
         </is>
       </c>
       <c r="C81" s="0">
-        <v>1793</v>
+        <v>762</v>
       </c>
       <c r="D81" s="1">
-        <v>41289.588722338</v>
+        <v>40917</v>
       </c>
       <c r="E81" s="0">
         <v>2</v>
@@ -1904,18 +1904,18 @@
     </row>
     <row outlineLevel="0" r="82">
       <c r="A82" s="0">
-        <v>185</v>
+        <v>101</v>
       </c>
       <c r="B82" s="0" t="inlineStr">
         <is>
-          <t>Sen. Phil Griego</t>
+          <t>NM Senate Majority Leadership Fund</t>
         </is>
       </c>
       <c r="C82" s="0">
-        <v>1793</v>
+        <v>1030</v>
       </c>
       <c r="D82" s="1">
-        <v>41289.5915252315</v>
+        <v>40921.4935462153</v>
       </c>
       <c r="E82" s="0">
         <v>2</v>
@@ -1923,18 +1923,18 @@
     </row>
     <row outlineLevel="0" r="83">
       <c r="A83" s="0">
-        <v>186</v>
+        <v>102</v>
       </c>
       <c r="B83" s="0" t="inlineStr">
         <is>
-          <t>Sen. Michael Sanchez</t>
+          <t>Comm to Elect Tom Taylor</t>
         </is>
       </c>
       <c r="C83" s="0">
-        <v>1793</v>
+        <v>1030</v>
       </c>
       <c r="D83" s="1">
-        <v>41289.5922797454</v>
+        <v>40921.5039724884</v>
       </c>
       <c r="E83" s="0">
         <v>2</v>
@@ -1942,18 +1942,18 @@
     </row>
     <row outlineLevel="0" r="84">
       <c r="A84" s="0">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="B84" s="0" t="inlineStr">
         <is>
-          <t>Sen. Richard Martinez</t>
+          <t>Governor Martinez PAC</t>
         </is>
       </c>
       <c r="C84" s="0">
-        <v>1793</v>
+        <v>1030</v>
       </c>
       <c r="D84" s="1">
-        <v>41289.5947354167</v>
+        <v>40921.5472732639</v>
       </c>
       <c r="E84" s="0">
         <v>2</v>
@@ -1961,18 +1961,18 @@
     </row>
     <row outlineLevel="0" r="85">
       <c r="A85" s="0">
-        <v>188</v>
+        <v>105</v>
       </c>
       <c r="B85" s="0" t="inlineStr">
         <is>
-          <t>Rep. Nick Salazar</t>
+          <t>Susana Martinez for Governor</t>
         </is>
       </c>
       <c r="C85" s="0">
-        <v>1793</v>
+        <v>1018</v>
       </c>
       <c r="D85" s="1">
-        <v>41289.6012427894</v>
+        <v>40924</v>
       </c>
       <c r="E85" s="0">
         <v>2</v>
@@ -1980,37 +1980,37 @@
     </row>
     <row outlineLevel="0" r="86">
       <c r="A86" s="0">
-        <v>189</v>
+        <v>109</v>
       </c>
       <c r="B86" s="0" t="inlineStr">
         <is>
-          <t>Rep. Debbie Rodella</t>
+          <t>andy nunez</t>
         </is>
       </c>
       <c r="C86" s="0">
-        <v>1793</v>
+        <v>1198</v>
       </c>
       <c r="D86" s="1">
-        <v>41289.6020223727</v>
+        <v>40963.3727584143</v>
       </c>
       <c r="E86" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="87">
       <c r="A87" s="0">
-        <v>190</v>
+        <v>111</v>
       </c>
       <c r="B87" s="0" t="inlineStr">
         <is>
-          <t>Rep. Ken Martinez</t>
+          <t>David Ulibarri</t>
         </is>
       </c>
       <c r="C87" s="0">
-        <v>1793</v>
+        <v>1048</v>
       </c>
       <c r="D87" s="1">
-        <v>41289.6031467245</v>
+        <v>40969.453783831</v>
       </c>
       <c r="E87" s="0">
         <v>2</v>
@@ -2018,18 +2018,18 @@
     </row>
     <row outlineLevel="0" r="88">
       <c r="A88" s="0">
-        <v>191</v>
+        <v>112</v>
       </c>
       <c r="B88" s="0" t="inlineStr">
         <is>
-          <t>v</t>
+          <t>Tom Taylor</t>
         </is>
       </c>
       <c r="C88" s="0">
-        <v>1847</v>
+        <v>1048</v>
       </c>
       <c r="D88" s="1">
-        <v>41289</v>
+        <v>40969.4551866551</v>
       </c>
       <c r="E88" s="0">
         <v>2</v>
@@ -2037,18 +2037,18 @@
     </row>
     <row outlineLevel="0" r="89">
       <c r="A89" s="0">
-        <v>192</v>
+        <v>113</v>
       </c>
       <c r="B89" s="0" t="inlineStr">
         <is>
-          <t>James Strickler Committee</t>
+          <t>Bill Sharer</t>
         </is>
       </c>
       <c r="C89" s="0">
-        <v>1943</v>
+        <v>1048</v>
       </c>
       <c r="D89" s="1">
-        <v>41391</v>
+        <v>40969.4562753125</v>
       </c>
       <c r="E89" s="0">
         <v>2</v>
@@ -2056,18 +2056,18 @@
     </row>
     <row outlineLevel="0" r="90">
       <c r="A90" s="0">
-        <v>193</v>
+        <v>115</v>
       </c>
       <c r="B90" s="0" t="inlineStr">
         <is>
-          <t>Various legislators</t>
+          <t>Debbie Rodella</t>
         </is>
       </c>
       <c r="C90" s="0">
-        <v>2184</v>
+        <v>1048</v>
       </c>
       <c r="D90" s="1">
-        <v>41395.5729660532</v>
+        <v>40969</v>
       </c>
       <c r="E90" s="0">
         <v>2</v>
@@ -2075,18 +2075,18 @@
     </row>
     <row outlineLevel="0" r="91">
       <c r="A91" s="0">
-        <v>194</v>
+        <v>116</v>
       </c>
       <c r="B91" s="0" t="inlineStr">
         <is>
-          <t>Representative Rick Miera and Rep. Miera</t>
+          <t>Henry Saavedra</t>
         </is>
       </c>
       <c r="C91" s="0">
-        <v>2250</v>
+        <v>1048</v>
       </c>
       <c r="D91" s="1">
-        <v>41403.5866740741</v>
+        <v>40969.4643073727</v>
       </c>
       <c r="E91" s="0">
         <v>2</v>
@@ -2094,18 +2094,18 @@
     </row>
     <row outlineLevel="0" r="92">
       <c r="A92" s="0">
-        <v>195</v>
+        <v>117</v>
       </c>
       <c r="B92" s="0" t="inlineStr">
         <is>
-          <t>Michael Padilla Committee</t>
+          <t>Bill Payne</t>
         </is>
       </c>
       <c r="C92" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D92" s="1">
-        <v>41647</v>
+        <v>40969.4652428588</v>
       </c>
       <c r="E92" s="0">
         <v>2</v>
@@ -2113,18 +2113,18 @@
     </row>
     <row outlineLevel="0" r="93">
       <c r="A93" s="0">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="B93" s="0" t="inlineStr">
         <is>
-          <t>Miguel Garcia Committee</t>
+          <t>John Ryan</t>
         </is>
       </c>
       <c r="C93" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D93" s="1">
-        <v>41647.4683474537</v>
+        <v>40969.4659270023</v>
       </c>
       <c r="E93" s="0">
         <v>2</v>
@@ -2132,18 +2132,18 @@
     </row>
     <row outlineLevel="0" r="94">
       <c r="A94" s="0">
-        <v>197</v>
+        <v>119</v>
       </c>
       <c r="B94" s="0" t="inlineStr">
         <is>
-          <t>Phil Griego Committee</t>
+          <t>Steve Neville</t>
         </is>
       </c>
       <c r="C94" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D94" s="1">
-        <v>41647.4858498032</v>
+        <v>40969.467762581</v>
       </c>
       <c r="E94" s="0">
         <v>2</v>
@@ -2151,18 +2151,18 @@
     </row>
     <row outlineLevel="0" r="95">
       <c r="A95" s="0">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="B95" s="0" t="inlineStr">
         <is>
-          <t>Nate Gentry Committee</t>
+          <t>Richard Martinez</t>
         </is>
       </c>
       <c r="C95" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D95" s="1">
-        <v>41647.4960348032</v>
+        <v>40969.4687997338</v>
       </c>
       <c r="E95" s="0">
         <v>2</v>
@@ -2170,18 +2170,18 @@
     </row>
     <row outlineLevel="0" r="96">
       <c r="A96" s="0">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B96" s="0" t="inlineStr">
         <is>
-          <t>John Sapien Committee</t>
+          <t>Stuart Ingle</t>
         </is>
       </c>
       <c r="C96" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D96" s="1">
-        <v>41647.5057917477</v>
+        <v>40969.4695037847</v>
       </c>
       <c r="E96" s="0">
         <v>2</v>
@@ -2189,18 +2189,18 @@
     </row>
     <row outlineLevel="0" r="97">
       <c r="A97" s="0">
-        <v>200</v>
+        <v>122</v>
       </c>
       <c r="B97" s="0" t="inlineStr">
         <is>
-          <t>Carroll Leavell Committee</t>
+          <t>Clint Harden</t>
         </is>
       </c>
       <c r="C97" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D97" s="1">
-        <v>41647.5065711806</v>
+        <v>40969</v>
       </c>
       <c r="E97" s="0">
         <v>2</v>
@@ -2208,18 +2208,18 @@
     </row>
     <row outlineLevel="0" r="98">
       <c r="A98" s="0">
-        <v>201</v>
+        <v>123</v>
       </c>
       <c r="B98" s="0" t="inlineStr">
         <is>
-          <t>Catherine Brown Committee</t>
+          <t>Carlos Cisneros</t>
         </is>
       </c>
       <c r="C98" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D98" s="1">
-        <v>41647.5075068634</v>
+        <v>40969.4711525116</v>
       </c>
       <c r="E98" s="0">
         <v>2</v>
@@ -2227,18 +2227,18 @@
     </row>
     <row outlineLevel="0" r="99">
       <c r="A99" s="0">
-        <v>202</v>
+        <v>124</v>
       </c>
       <c r="B99" s="0" t="inlineStr">
         <is>
-          <t>Zach Cook Committee</t>
+          <t>Vernon Asbill</t>
         </is>
       </c>
       <c r="C99" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D99" s="1">
-        <v>41647.5082868403</v>
+        <v>40969</v>
       </c>
       <c r="E99" s="0">
         <v>2</v>
@@ -2246,18 +2246,18 @@
     </row>
     <row outlineLevel="0" r="100">
       <c r="A100" s="0">
-        <v>203</v>
+        <v>125</v>
       </c>
       <c r="B100" s="0" t="inlineStr">
         <is>
-          <t>Brian Egolf Committee</t>
+          <t>Rod Adair</t>
         </is>
       </c>
       <c r="C100" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D100" s="1">
-        <v>41647.5089691782</v>
+        <v>40969.4731597222</v>
       </c>
       <c r="E100" s="0">
         <v>2</v>
@@ -2265,18 +2265,18 @@
     </row>
     <row outlineLevel="0" r="101">
       <c r="A101" s="0">
-        <v>204</v>
+        <v>126</v>
       </c>
       <c r="B101" s="0" t="inlineStr">
         <is>
-          <t>Kelly Fajardo Committee</t>
+          <t>Phil Griego</t>
         </is>
       </c>
       <c r="C101" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D101" s="1">
-        <v>41647.5096247338</v>
+        <v>40969.4739550926</v>
       </c>
       <c r="E101" s="0">
         <v>2</v>
@@ -2284,18 +2284,18 @@
     </row>
     <row outlineLevel="0" r="102">
       <c r="A102" s="0">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="B102" s="0" t="inlineStr">
         <is>
-          <t>Terry McMillian Committee</t>
+          <t>Susana Martinez</t>
         </is>
       </c>
       <c r="C102" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D102" s="1">
-        <v>41647.5103475694</v>
+        <v>40969.4746129977</v>
       </c>
       <c r="E102" s="0">
         <v>2</v>
@@ -2303,18 +2303,18 @@
     </row>
     <row outlineLevel="0" r="103">
       <c r="A103" s="0">
-        <v>206</v>
+        <v>129</v>
       </c>
       <c r="B103" s="0" t="inlineStr">
         <is>
-          <t>Bill Rehm Committee</t>
+          <t>Tim Lewis</t>
         </is>
       </c>
       <c r="C103" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D103" s="1">
-        <v>41647.5109582986</v>
+        <v>40969.5033022338</v>
       </c>
       <c r="E103" s="0">
         <v>2</v>
@@ -2322,18 +2322,18 @@
     </row>
     <row outlineLevel="0" r="104">
       <c r="A104" s="0">
-        <v>207</v>
+        <v>130</v>
       </c>
       <c r="B104" s="0" t="inlineStr">
         <is>
-          <t>Susana Martinez Committee</t>
+          <t>Michael Sanchez</t>
         </is>
       </c>
       <c r="C104" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D104" s="1">
-        <v>41647.5116151273</v>
+        <v>40969</v>
       </c>
       <c r="E104" s="0">
         <v>2</v>
@@ -2341,18 +2341,18 @@
     </row>
     <row outlineLevel="0" r="105">
       <c r="A105" s="0">
-        <v>208</v>
+        <v>131</v>
       </c>
       <c r="B105" s="0" t="inlineStr">
         <is>
-          <t>Bobby Gonzales Committee</t>
+          <t>Stuart Ingle</t>
         </is>
       </c>
       <c r="C105" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D105" s="1">
-        <v>41647.5981723727</v>
+        <v>40969.5283819792</v>
       </c>
       <c r="E105" s="0">
         <v>2</v>
@@ -2360,18 +2360,18 @@
     </row>
     <row outlineLevel="0" r="106">
       <c r="A106" s="0">
-        <v>209</v>
+        <v>132</v>
       </c>
       <c r="B106" s="0" t="inlineStr">
         <is>
-          <t>Debbie Rodella Committee</t>
+          <t>Bill Sharer</t>
         </is>
       </c>
       <c r="C106" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D106" s="1">
-        <v>41647.6055184838</v>
+        <v>40969.5291003125</v>
       </c>
       <c r="E106" s="0">
         <v>2</v>
@@ -2379,18 +2379,18 @@
     </row>
     <row outlineLevel="0" r="107">
       <c r="A107" s="0">
-        <v>210</v>
+        <v>133</v>
       </c>
       <c r="B107" s="0" t="inlineStr">
         <is>
-          <t>Ken Martinez Committee</t>
+          <t>Bill Payne</t>
         </is>
       </c>
       <c r="C107" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D107" s="1">
-        <v>41647.6099128472</v>
+        <v>40969.5297082986</v>
       </c>
       <c r="E107" s="0">
         <v>2</v>
@@ -2398,18 +2398,18 @@
     </row>
     <row outlineLevel="0" r="108">
       <c r="A108" s="0">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="B108" s="0" t="inlineStr">
         <is>
-          <t>Doreen Gallegos Committee</t>
+          <t>Steve Neville</t>
         </is>
       </c>
       <c r="C108" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D108" s="1">
-        <v>41647.613925081</v>
+        <v>40969.5303155903</v>
       </c>
       <c r="E108" s="0">
         <v>2</v>
@@ -2417,18 +2417,18 @@
     </row>
     <row outlineLevel="0" r="109">
       <c r="A109" s="0">
-        <v>212</v>
+        <v>135</v>
       </c>
       <c r="B109" s="0" t="inlineStr">
         <is>
-          <t>Rick Miera Committee</t>
+          <t>Phil Griego</t>
         </is>
       </c>
       <c r="C109" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D109" s="1">
-        <v>41647.6175880787</v>
+        <v>40969.5310568634</v>
       </c>
       <c r="E109" s="0">
         <v>2</v>
@@ -2436,18 +2436,18 @@
     </row>
     <row outlineLevel="0" r="110">
       <c r="A110" s="0">
-        <v>213</v>
+        <v>136</v>
       </c>
       <c r="B110" s="0" t="inlineStr">
         <is>
-          <t>Tom Taylor Commitee</t>
+          <t>David Ulibarri</t>
         </is>
       </c>
       <c r="C110" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D110" s="1">
-        <v>41647.618943669</v>
+        <v>40969.5316287037</v>
       </c>
       <c r="E110" s="0">
         <v>2</v>
@@ -2455,18 +2455,18 @@
     </row>
     <row outlineLevel="0" r="111">
       <c r="A111" s="0">
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="B111" s="0" t="inlineStr">
         <is>
-          <t>Rudy Martinez Committee</t>
+          <t>Richard Martinez</t>
         </is>
       </c>
       <c r="C111" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D111" s="1">
-        <v>41647.6198285532</v>
+        <v>40969.5321478819</v>
       </c>
       <c r="E111" s="0">
         <v>2</v>
@@ -2474,18 +2474,18 @@
     </row>
     <row outlineLevel="0" r="112">
       <c r="A112" s="0">
-        <v>215</v>
+        <v>138</v>
       </c>
       <c r="B112" s="0" t="inlineStr">
         <is>
-          <t>Bill Sharer Committee</t>
+          <t>George Munoz</t>
         </is>
       </c>
       <c r="C112" s="0">
-        <v>2351</v>
+        <v>1048</v>
       </c>
       <c r="D112" s="1">
-        <v>41647.6209264699</v>
+        <v>40969.532846331</v>
       </c>
       <c r="E112" s="0">
         <v>2</v>
@@ -2493,18 +2493,18 @@
     </row>
     <row outlineLevel="0" r="113">
       <c r="A113" s="0">
-        <v>216</v>
+        <v>139</v>
       </c>
       <c r="B113" s="0" t="inlineStr">
         <is>
-          <t>Hector Balderos Committee</t>
+          <t>Susana PAC</t>
         </is>
       </c>
       <c r="C113" s="0">
-        <v>2351</v>
+        <v>1270</v>
       </c>
       <c r="D113" s="1">
-        <v>41647.6218800579</v>
+        <v>41022</v>
       </c>
       <c r="E113" s="0">
         <v>2</v>
@@ -2512,56 +2512,56 @@
     </row>
     <row outlineLevel="0" r="114">
       <c r="A114" s="0">
-        <v>217</v>
+        <v>140</v>
       </c>
       <c r="B114" s="0" t="inlineStr">
         <is>
-          <t>Mary Kay Papen Committee</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C114" s="0">
-        <v>2351</v>
+        <v>1271</v>
       </c>
       <c r="D114" s="1">
-        <v>41647.6244457176</v>
+        <v>41022.364206794</v>
       </c>
       <c r="E114" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="115">
       <c r="A115" s="0">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="B115" s="0" t="inlineStr">
         <is>
-          <t>Michael Sanchez Committee</t>
+          <t>Jane Doe</t>
         </is>
       </c>
       <c r="C115" s="0">
-        <v>2351</v>
+        <v>1271</v>
       </c>
       <c r="D115" s="1">
-        <v>41647.6254394676</v>
+        <v>41022.3665546644</v>
       </c>
       <c r="E115" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="116">
       <c r="A116" s="0">
-        <v>219</v>
+        <v>142</v>
       </c>
       <c r="B116" s="0" t="inlineStr">
         <is>
-          <t>Steve Neville Committee</t>
+          <t>Phil Griego Committee</t>
         </is>
       </c>
       <c r="C116" s="0">
-        <v>2351</v>
+        <v>1270</v>
       </c>
       <c r="D116" s="1">
-        <v>41647.6273356134</v>
+        <v>41022.5227876968</v>
       </c>
       <c r="E116" s="0">
         <v>2</v>
@@ -2569,37 +2569,37 @@
     </row>
     <row outlineLevel="0" r="117">
       <c r="A117" s="0">
-        <v>220</v>
+        <v>143</v>
       </c>
       <c r="B117" s="0" t="inlineStr">
         <is>
-          <t>Mark Moores Committee</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C117" s="0">
-        <v>2351</v>
+        <v>1313</v>
       </c>
       <c r="D117" s="1">
-        <v>41647.7168352199</v>
+        <v>41024.7078077894</v>
       </c>
       <c r="E117" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="118">
       <c r="A118" s="0">
-        <v>221</v>
+        <v>144</v>
       </c>
       <c r="B118" s="0" t="inlineStr">
         <is>
-          <t>Christine Trujillo Committee</t>
+          <t>Legislature</t>
         </is>
       </c>
       <c r="C118" s="0">
-        <v>2351</v>
+        <v>1367</v>
       </c>
       <c r="D118" s="1">
-        <v>41647.7179861111</v>
+        <v>41026.4807114236</v>
       </c>
       <c r="E118" s="0">
         <v>2</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row outlineLevel="0" r="119">
       <c r="A119" s="0">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="B119" s="0" t="inlineStr">
         <is>
@@ -2615,10 +2615,10 @@
         </is>
       </c>
       <c r="C119" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D119" s="1">
-        <v>41647.7189679051</v>
+        <v>41282</v>
       </c>
       <c r="E119" s="0">
         <v>2</v>
@@ -2626,18 +2626,18 @@
     </row>
     <row outlineLevel="0" r="120">
       <c r="A120" s="0">
-        <v>223</v>
+        <v>157</v>
       </c>
       <c r="B120" s="0" t="inlineStr">
         <is>
-          <t>Michael Sanchez Committee</t>
+          <t>Tom Taylor Committee</t>
         </is>
       </c>
       <c r="C120" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D120" s="1">
-        <v>41647.720497338</v>
+        <v>41282</v>
       </c>
       <c r="E120" s="0">
         <v>2</v>
@@ -2645,18 +2645,18 @@
     </row>
     <row outlineLevel="0" r="121">
       <c r="A121" s="0">
-        <v>224</v>
+        <v>158</v>
       </c>
       <c r="B121" s="0" t="inlineStr">
         <is>
-          <t>Howie Morales Committee</t>
+          <t>Carl Trujillo Committee</t>
         </is>
       </c>
       <c r="C121" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D121" s="1">
-        <v>41647.7212693634</v>
+        <v>41282.581194294</v>
       </c>
       <c r="E121" s="0">
         <v>2</v>
@@ -2664,18 +2664,18 @@
     </row>
     <row outlineLevel="0" r="122">
       <c r="A122" s="0">
-        <v>225</v>
+        <v>159</v>
       </c>
       <c r="B122" s="0" t="inlineStr">
         <is>
-          <t>Sander Rue Committee</t>
+          <t>Nancy Rodiguez Committee</t>
         </is>
       </c>
       <c r="C122" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D122" s="1">
-        <v>41647.7222477199</v>
+        <v>41282</v>
       </c>
       <c r="E122" s="0">
         <v>2</v>
@@ -2683,18 +2683,18 @@
     </row>
     <row outlineLevel="0" r="123">
       <c r="A123" s="0">
-        <v>226</v>
+        <v>160</v>
       </c>
       <c r="B123" s="0" t="inlineStr">
         <is>
-          <t>Alonzo Baldonado Committee</t>
+          <t>Phil Griego Committee</t>
         </is>
       </c>
       <c r="C123" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D123" s="1">
-        <v>41648.6875886227</v>
+        <v>41282</v>
       </c>
       <c r="E123" s="0">
         <v>2</v>
@@ -2702,18 +2702,18 @@
     </row>
     <row outlineLevel="0" r="124">
       <c r="A124" s="0">
-        <v>227</v>
+        <v>162</v>
       </c>
       <c r="B124" s="0" t="inlineStr">
         <is>
-          <t>Gail Chasey Committee</t>
+          <t>Governor Susana Martinez</t>
         </is>
       </c>
       <c r="C124" s="0">
-        <v>2351</v>
+        <v>1600</v>
       </c>
       <c r="D124" s="1">
-        <v>41648.6884904745</v>
+        <v>41283</v>
       </c>
       <c r="E124" s="0">
         <v>2</v>
@@ -2721,18 +2721,18 @@
     </row>
     <row outlineLevel="0" r="125">
       <c r="A125" s="0">
-        <v>228</v>
+        <v>163</v>
       </c>
       <c r="B125" s="0" t="inlineStr">
         <is>
-          <t>Ernest Chavez Committee</t>
+          <t>Paul Pacheco Committee</t>
         </is>
       </c>
       <c r="C125" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D125" s="1">
-        <v>41648.6893207523</v>
+        <v>41283</v>
       </c>
       <c r="E125" s="0">
         <v>2</v>
@@ -2740,18 +2740,18 @@
     </row>
     <row outlineLevel="0" r="126">
       <c r="A126" s="0">
-        <v>229</v>
+        <v>164</v>
       </c>
       <c r="B126" s="0" t="inlineStr">
         <is>
-          <t>Sharon Clahchischilliage Committee</t>
+          <t>Tom Taylor Committee</t>
         </is>
       </c>
       <c r="C126" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D126" s="1">
-        <v>41648.6903244213</v>
+        <v>41283.4961366088</v>
       </c>
       <c r="E126" s="0">
         <v>2</v>
@@ -2759,18 +2759,18 @@
     </row>
     <row outlineLevel="0" r="127">
       <c r="A127" s="0">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="B127" s="0" t="inlineStr">
         <is>
-          <t>Stephanie Garcia Richard Committee</t>
+          <t>Ken Martinez Committee</t>
         </is>
       </c>
       <c r="C127" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D127" s="1">
-        <v>41648.6926665509</v>
+        <v>41283.4972309028</v>
       </c>
       <c r="E127" s="0">
         <v>2</v>
@@ -2778,18 +2778,18 @@
     </row>
     <row outlineLevel="0" r="128">
       <c r="A128" s="0">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="B128" s="0" t="inlineStr">
         <is>
-          <t>Jason Harper Committee</t>
+          <t>Michael Sanchez Committee</t>
         </is>
       </c>
       <c r="C128" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D128" s="1">
-        <v>41648.6935905093</v>
+        <v>41283.4980327546</v>
       </c>
       <c r="E128" s="0">
         <v>2</v>
@@ -2797,18 +2797,18 @@
     </row>
     <row outlineLevel="0" r="129">
       <c r="A129" s="0">
-        <v>232</v>
+        <v>167</v>
       </c>
       <c r="B129" s="0" t="inlineStr">
         <is>
-          <t>Georgene Louis Committee</t>
+          <t>Lee Alcon Committee</t>
         </is>
       </c>
       <c r="C129" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D129" s="1">
-        <v>41648.6945314468</v>
+        <v>41283</v>
       </c>
       <c r="E129" s="0">
         <v>2</v>
@@ -2816,18 +2816,18 @@
     </row>
     <row outlineLevel="0" r="130">
       <c r="A130" s="0">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="B130" s="0" t="inlineStr">
         <is>
-          <t>James Smith Committee</t>
+          <t>Lynda Lovejoy Committee</t>
         </is>
       </c>
       <c r="C130" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D130" s="1">
-        <v>41648.6987031597</v>
+        <v>41283</v>
       </c>
       <c r="E130" s="0">
         <v>2</v>
@@ -2835,18 +2835,18 @@
     </row>
     <row outlineLevel="0" r="131">
       <c r="A131" s="0">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="B131" s="0" t="inlineStr">
         <is>
-          <t>Carl Trujillo Committee</t>
+          <t>Yvette Herrell  Committee</t>
         </is>
       </c>
       <c r="C131" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D131" s="1">
-        <v>41648.6997956366</v>
+        <v>41283</v>
       </c>
       <c r="E131" s="0">
         <v>2</v>
@@ -2854,18 +2854,18 @@
     </row>
     <row outlineLevel="0" r="132">
       <c r="A132" s="0">
-        <v>235</v>
+        <v>170</v>
       </c>
       <c r="B132" s="0" t="inlineStr">
         <is>
-          <t>Jim Trujillo Committee</t>
+          <t>Larry Larranga Committee</t>
         </is>
       </c>
       <c r="C132" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D132" s="1">
-        <v>41648.7022064815</v>
+        <v>41283</v>
       </c>
       <c r="E132" s="0">
         <v>2</v>
@@ -2873,18 +2873,18 @@
     </row>
     <row outlineLevel="0" r="133">
       <c r="A133" s="0">
-        <v>236</v>
+        <v>171</v>
       </c>
       <c r="B133" s="0" t="inlineStr">
         <is>
-          <t>Jacob Candelaria Committee</t>
+          <t>House R Leadership Fund</t>
         </is>
       </c>
       <c r="C133" s="0">
-        <v>2351</v>
+        <v>1614</v>
       </c>
       <c r="D133" s="1">
-        <v>41648.7032034722</v>
+        <v>41283</v>
       </c>
       <c r="E133" s="0">
         <v>2</v>
@@ -2892,18 +2892,18 @@
     </row>
     <row outlineLevel="0" r="134">
       <c r="A134" s="0">
-        <v>237</v>
+        <v>172</v>
       </c>
       <c r="B134" s="0" t="inlineStr">
         <is>
-          <t>Joseph Cervantes Committee</t>
+          <t>ReElect Sen. Richard C. Martinez</t>
         </is>
       </c>
       <c r="C134" s="0">
-        <v>2351</v>
+        <v>1702</v>
       </c>
       <c r="D134" s="1">
-        <v>41648.7039840278</v>
+        <v>41284.4519641551</v>
       </c>
       <c r="E134" s="0">
         <v>2</v>
@@ -2911,18 +2911,18 @@
     </row>
     <row outlineLevel="0" r="135">
       <c r="A135" s="0">
-        <v>238</v>
+        <v>173</v>
       </c>
       <c r="B135" s="0" t="inlineStr">
         <is>
-          <t>Carlos Cisneros Committee</t>
+          <t>Rep. Ray Begaye</t>
         </is>
       </c>
       <c r="C135" s="0">
-        <v>2351</v>
+        <v>1793</v>
       </c>
       <c r="D135" s="1">
-        <v>41648.7047381597</v>
+        <v>41289</v>
       </c>
       <c r="E135" s="0">
         <v>2</v>
@@ -2930,18 +2930,18 @@
     </row>
     <row outlineLevel="0" r="136">
       <c r="A136" s="0">
-        <v>239</v>
+        <v>174</v>
       </c>
       <c r="B136" s="0" t="inlineStr">
         <is>
-          <t>Stuart Ingle Committee</t>
+          <t>Sen. Tim Jennings</t>
         </is>
       </c>
       <c r="C136" s="0">
-        <v>2351</v>
+        <v>1793</v>
       </c>
       <c r="D136" s="1">
-        <v>41648.7054517361</v>
+        <v>41289.5752457523</v>
       </c>
       <c r="E136" s="0">
         <v>2</v>
@@ -2949,18 +2949,18 @@
     </row>
     <row outlineLevel="0" r="137">
       <c r="A137" s="0">
-        <v>240</v>
+        <v>175</v>
       </c>
       <c r="B137" s="0" t="inlineStr">
         <is>
-          <t>Richard Martinez Committee</t>
+          <t>Rep. Tim Lewis</t>
         </is>
       </c>
       <c r="C137" s="0">
-        <v>2351</v>
+        <v>1793</v>
       </c>
       <c r="D137" s="1">
-        <v>41648.7062680903</v>
+        <v>41289.576412581</v>
       </c>
       <c r="E137" s="0">
         <v>2</v>
@@ -2968,18 +2968,18 @@
     </row>
     <row outlineLevel="0" r="138">
       <c r="A138" s="0">
-        <v>241</v>
+        <v>176</v>
       </c>
       <c r="B138" s="0" t="inlineStr">
         <is>
-          <t>Lisa Torraco Committee</t>
+          <t>Rep. Nate Gentry</t>
         </is>
       </c>
       <c r="C138" s="0">
-        <v>2351</v>
+        <v>1793</v>
       </c>
       <c r="D138" s="1">
-        <v>41648.70776875</v>
+        <v>41289.5773395833</v>
       </c>
       <c r="E138" s="0">
         <v>2</v>
@@ -2987,18 +2987,18 @@
     </row>
     <row outlineLevel="0" r="139">
       <c r="A139" s="0">
-        <v>242</v>
+        <v>177</v>
       </c>
       <c r="B139" s="0" t="inlineStr">
         <is>
-          <t>Bill Payne Committee</t>
+          <t>Rep. Alonzo Baldonado</t>
         </is>
       </c>
       <c r="C139" s="0">
-        <v>2351</v>
+        <v>1793</v>
       </c>
       <c r="D139" s="1">
-        <v>41648.7086337153</v>
+        <v>41289.578472419</v>
       </c>
       <c r="E139" s="0">
         <v>2</v>
@@ -3006,18 +3006,18 @@
     </row>
     <row outlineLevel="0" r="140">
       <c r="A140" s="0">
-        <v>243</v>
+        <v>178</v>
       </c>
       <c r="B140" s="0" t="inlineStr">
         <is>
-          <t>Gary King Committee</t>
+          <t>Rep. Conrad James</t>
         </is>
       </c>
       <c r="C140" s="0">
-        <v>2351</v>
+        <v>1793</v>
       </c>
       <c r="D140" s="1">
-        <v>41648.7224611111</v>
+        <v>41289.5793075579</v>
       </c>
       <c r="E140" s="0">
         <v>2</v>
@@ -3025,18 +3025,18 @@
     </row>
     <row outlineLevel="0" r="141">
       <c r="A141" s="0">
-        <v>244</v>
+        <v>179</v>
       </c>
       <c r="B141" s="0" t="inlineStr">
         <is>
-          <t>Re-elect State Representative Sandra Jeff</t>
+          <t>Rep. Ed Sandoval</t>
         </is>
       </c>
       <c r="C141" s="0">
-        <v>2401</v>
+        <v>1793</v>
       </c>
       <c r="D141" s="1">
-        <v>41653</v>
+        <v>41289.5827920486</v>
       </c>
       <c r="E141" s="0">
         <v>2</v>
@@ -3044,18 +3044,18 @@
     </row>
     <row outlineLevel="0" r="142">
       <c r="A142" s="0">
-        <v>245</v>
+        <v>180</v>
       </c>
       <c r="B142" s="0" t="inlineStr">
         <is>
-          <t>Munoz for Senate</t>
+          <t>Marci Blaze</t>
         </is>
       </c>
       <c r="C142" s="0">
-        <v>2401</v>
+        <v>1793</v>
       </c>
       <c r="D142" s="1">
-        <v>41653</v>
+        <v>41289.5839465625</v>
       </c>
       <c r="E142" s="0">
         <v>2</v>
@@ -3063,18 +3063,18 @@
     </row>
     <row outlineLevel="0" r="143">
       <c r="A143" s="0">
-        <v>246</v>
+        <v>181</v>
       </c>
       <c r="B143" s="0" t="inlineStr">
         <is>
-          <t>Michael Padilla</t>
+          <t>Clemente Sanchez</t>
         </is>
       </c>
       <c r="C143" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D143" s="1">
-        <v>41661</v>
+        <v>41289.5850884259</v>
       </c>
       <c r="E143" s="0">
         <v>2</v>
@@ -3082,18 +3082,18 @@
     </row>
     <row outlineLevel="0" r="144">
       <c r="A144" s="0">
-        <v>247</v>
+        <v>182</v>
       </c>
       <c r="B144" s="0" t="inlineStr">
         <is>
-          <t>Emily Kane</t>
+          <t>Bill McCamley</t>
         </is>
       </c>
       <c r="C144" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D144" s="1">
-        <v>41661</v>
+        <v>41289.5863151273</v>
       </c>
       <c r="E144" s="0">
         <v>2</v>
@@ -3101,18 +3101,18 @@
     </row>
     <row outlineLevel="0" r="145">
       <c r="A145" s="0">
-        <v>248</v>
+        <v>183</v>
       </c>
       <c r="B145" s="0" t="inlineStr">
         <is>
-          <t>Lisa Torraco</t>
+          <t>Stephen Easley</t>
         </is>
       </c>
       <c r="C145" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D145" s="1">
-        <v>41661.6273397801</v>
+        <v>41289.5879890046</v>
       </c>
       <c r="E145" s="0">
         <v>2</v>
@@ -3120,18 +3120,18 @@
     </row>
     <row outlineLevel="0" r="146">
       <c r="A146" s="0">
-        <v>249</v>
+        <v>184</v>
       </c>
       <c r="B146" s="0" t="inlineStr">
         <is>
-          <t>Mark Moores</t>
+          <t>Jeff Steinborn</t>
         </is>
       </c>
       <c r="C146" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D146" s="1">
-        <v>41661.6283504977</v>
+        <v>41289.588722338</v>
       </c>
       <c r="E146" s="0">
         <v>2</v>
@@ -3139,18 +3139,18 @@
     </row>
     <row outlineLevel="0" r="147">
       <c r="A147" s="0">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="B147" s="0" t="inlineStr">
         <is>
-          <t>Nate Gentry</t>
+          <t>Sen. Phil Griego</t>
         </is>
       </c>
       <c r="C147" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D147" s="1">
-        <v>41661.6289706366</v>
+        <v>41289.5915252315</v>
       </c>
       <c r="E147" s="0">
         <v>2</v>
@@ -3158,18 +3158,18 @@
     </row>
     <row outlineLevel="0" r="148">
       <c r="A148" s="0">
-        <v>251</v>
+        <v>186</v>
       </c>
       <c r="B148" s="0" t="inlineStr">
         <is>
-          <t>Carl Trujillo</t>
+          <t>Sen. Michael Sanchez</t>
         </is>
       </c>
       <c r="C148" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D148" s="1">
-        <v>41661.6298482639</v>
+        <v>41289.5922797454</v>
       </c>
       <c r="E148" s="0">
         <v>2</v>
@@ -3177,18 +3177,18 @@
     </row>
     <row outlineLevel="0" r="149">
       <c r="A149" s="0">
-        <v>252</v>
+        <v>187</v>
       </c>
       <c r="B149" s="0" t="inlineStr">
         <is>
-          <t>John Sapien</t>
+          <t>Sen. Richard Martinez</t>
         </is>
       </c>
       <c r="C149" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D149" s="1">
-        <v>41661.6392118866</v>
+        <v>41289.5947354167</v>
       </c>
       <c r="E149" s="0">
         <v>2</v>
@@ -3196,18 +3196,18 @@
     </row>
     <row outlineLevel="0" r="150">
       <c r="A150" s="0">
-        <v>253</v>
+        <v>188</v>
       </c>
       <c r="B150" s="0" t="inlineStr">
         <is>
-          <t>Phil Griego</t>
+          <t>Rep. Nick Salazar</t>
         </is>
       </c>
       <c r="C150" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D150" s="1">
-        <v>41661.6401135764</v>
+        <v>41289.6012427894</v>
       </c>
       <c r="E150" s="0">
         <v>2</v>
@@ -3215,18 +3215,18 @@
     </row>
     <row outlineLevel="0" r="151">
       <c r="A151" s="0">
-        <v>254</v>
+        <v>189</v>
       </c>
       <c r="B151" s="0" t="inlineStr">
         <is>
-          <t>Pete Campos</t>
+          <t>Rep. Debbie Rodella</t>
         </is>
       </c>
       <c r="C151" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D151" s="1">
-        <v>41661.6407568287</v>
+        <v>41289.6020223727</v>
       </c>
       <c r="E151" s="0">
         <v>2</v>
@@ -3234,18 +3234,18 @@
     </row>
     <row outlineLevel="0" r="152">
       <c r="A152" s="0">
-        <v>255</v>
+        <v>190</v>
       </c>
       <c r="B152" s="0" t="inlineStr">
         <is>
-          <t>Stephanie Garcia-Richard</t>
+          <t>Rep. Ken Martinez</t>
         </is>
       </c>
       <c r="C152" s="0">
-        <v>2515</v>
+        <v>1793</v>
       </c>
       <c r="D152" s="1">
-        <v>41661.6415364583</v>
+        <v>41289.6031467245</v>
       </c>
       <c r="E152" s="0">
         <v>2</v>
@@ -3253,18 +3253,18 @@
     </row>
     <row outlineLevel="0" r="153">
       <c r="A153" s="0">
-        <v>256</v>
+        <v>191</v>
       </c>
       <c r="B153" s="0" t="inlineStr">
         <is>
-          <t>Monica Youngblood</t>
+          <t>v</t>
         </is>
       </c>
       <c r="C153" s="0">
-        <v>2515</v>
+        <v>1847</v>
       </c>
       <c r="D153" s="1">
-        <v>41661.6422158912</v>
+        <v>41289</v>
       </c>
       <c r="E153" s="0">
         <v>2</v>
@@ -3272,18 +3272,18 @@
     </row>
     <row outlineLevel="0" r="154">
       <c r="A154" s="0">
-        <v>266</v>
+        <v>192</v>
       </c>
       <c r="B154" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Luciano Varela</t>
+          <t>James Strickler Committee</t>
         </is>
       </c>
       <c r="C154" s="0">
-        <v>3012</v>
+        <v>1943</v>
       </c>
       <c r="D154" s="1">
-        <v>41995.2755185185</v>
+        <v>41391</v>
       </c>
       <c r="E154" s="0">
         <v>2</v>
@@ -3291,18 +3291,18 @@
     </row>
     <row outlineLevel="0" r="155">
       <c r="A155" s="0">
-        <v>267</v>
+        <v>193</v>
       </c>
       <c r="B155" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Rodney Montoya</t>
+          <t>Various legislators</t>
         </is>
       </c>
       <c r="C155" s="0">
-        <v>3012</v>
+        <v>2184</v>
       </c>
       <c r="D155" s="1">
-        <v>41995</v>
+        <v>41395.5729660532</v>
       </c>
       <c r="E155" s="0">
         <v>2</v>
@@ -3310,18 +3310,18 @@
     </row>
     <row outlineLevel="0" r="156">
       <c r="A156" s="0">
-        <v>268</v>
+        <v>194</v>
       </c>
       <c r="B156" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect James Strickler</t>
+          <t>Representative Rick Miera and Rep. Miera</t>
         </is>
       </c>
       <c r="C156" s="0">
-        <v>3012</v>
+        <v>2250</v>
       </c>
       <c r="D156" s="1">
-        <v>41995</v>
+        <v>41403.5866740741</v>
       </c>
       <c r="E156" s="0">
         <v>2</v>
@@ -3329,18 +3329,18 @@
     </row>
     <row outlineLevel="0" r="157">
       <c r="A157" s="0">
-        <v>269</v>
+        <v>195</v>
       </c>
       <c r="B157" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Paul Bandy</t>
+          <t>Michael Padilla Committee</t>
         </is>
       </c>
       <c r="C157" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D157" s="1">
-        <v>41995</v>
+        <v>41647</v>
       </c>
       <c r="E157" s="0">
         <v>2</v>
@@ -3348,18 +3348,18 @@
     </row>
     <row outlineLevel="0" r="158">
       <c r="A158" s="0">
-        <v>270</v>
+        <v>196</v>
       </c>
       <c r="B158" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Sharon Clahchischilliage</t>
+          <t>Miguel Garcia Committee</t>
         </is>
       </c>
       <c r="C158" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D158" s="1">
-        <v>41995.2819042824</v>
+        <v>41647.4683474537</v>
       </c>
       <c r="E158" s="0">
         <v>2</v>
@@ -3367,18 +3367,18 @@
     </row>
     <row outlineLevel="0" r="159">
       <c r="A159" s="0">
-        <v>271</v>
+        <v>197</v>
       </c>
       <c r="B159" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Kelly Fajardo</t>
+          <t>Phil Griego Committee</t>
         </is>
       </c>
       <c r="C159" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D159" s="1">
-        <v>41995</v>
+        <v>41647.4858498032</v>
       </c>
       <c r="E159" s="0">
         <v>2</v>
@@ -3386,18 +3386,18 @@
     </row>
     <row outlineLevel="0" r="160">
       <c r="A160" s="0">
-        <v>272</v>
+        <v>198</v>
       </c>
       <c r="B160" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Alonzo Baldonado</t>
+          <t>Nate Gentry Committee</t>
         </is>
       </c>
       <c r="C160" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D160" s="1">
-        <v>41995</v>
+        <v>41647.4960348032</v>
       </c>
       <c r="E160" s="0">
         <v>2</v>
@@ -3405,18 +3405,18 @@
     </row>
     <row outlineLevel="0" r="161">
       <c r="A161" s="0">
-        <v>273</v>
+        <v>199</v>
       </c>
       <c r="B161" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Sarah Maestas-Barnes</t>
+          <t>John Sapien Committee</t>
         </is>
       </c>
       <c r="C161" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D161" s="1">
-        <v>41995</v>
+        <v>41647.5057917477</v>
       </c>
       <c r="E161" s="0">
         <v>2</v>
@@ -3424,18 +3424,18 @@
     </row>
     <row outlineLevel="0" r="162">
       <c r="A162" s="0">
-        <v>274</v>
+        <v>200</v>
       </c>
       <c r="B162" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect James Smith</t>
+          <t>Carroll Leavell Committee</t>
         </is>
       </c>
       <c r="C162" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D162" s="1">
-        <v>41995</v>
+        <v>41647.5065711806</v>
       </c>
       <c r="E162" s="0">
         <v>2</v>
@@ -3443,18 +3443,18 @@
     </row>
     <row outlineLevel="0" r="163">
       <c r="A163" s="0">
-        <v>275</v>
+        <v>201</v>
       </c>
       <c r="B163" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Paul Pacheco</t>
+          <t>Catherine Brown Committee</t>
         </is>
       </c>
       <c r="C163" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D163" s="1">
-        <v>41995</v>
+        <v>41647.5075068634</v>
       </c>
       <c r="E163" s="0">
         <v>2</v>
@@ -3462,18 +3462,18 @@
     </row>
     <row outlineLevel="0" r="164">
       <c r="A164" s="0">
-        <v>276</v>
+        <v>202</v>
       </c>
       <c r="B164" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Conrad James</t>
+          <t>Zach Cook Committee</t>
         </is>
       </c>
       <c r="C164" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D164" s="1">
-        <v>41995</v>
+        <v>41647.5082868403</v>
       </c>
       <c r="E164" s="0">
         <v>2</v>
@@ -3481,18 +3481,18 @@
     </row>
     <row outlineLevel="0" r="165">
       <c r="A165" s="0">
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="B165" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Lorenzo Larranaga</t>
+          <t>Brian Egolf Committee</t>
         </is>
       </c>
       <c r="C165" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D165" s="1">
-        <v>41995</v>
+        <v>41647.5089691782</v>
       </c>
       <c r="E165" s="0">
         <v>2</v>
@@ -3500,18 +3500,18 @@
     </row>
     <row outlineLevel="0" r="166">
       <c r="A166" s="0">
-        <v>278</v>
+        <v>204</v>
       </c>
       <c r="B166" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Jimmie Hall</t>
+          <t>Kelly Fajardo Committee</t>
         </is>
       </c>
       <c r="C166" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D166" s="1">
-        <v>41995</v>
+        <v>41647.5096247338</v>
       </c>
       <c r="E166" s="0">
         <v>2</v>
@@ -3519,18 +3519,18 @@
     </row>
     <row outlineLevel="0" r="167">
       <c r="A167" s="0">
-        <v>279</v>
+        <v>205</v>
       </c>
       <c r="B167" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Nate Gentry</t>
+          <t>Terry McMillian Committee</t>
         </is>
       </c>
       <c r="C167" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D167" s="1">
-        <v>41995</v>
+        <v>41647.5103475694</v>
       </c>
       <c r="E167" s="0">
         <v>2</v>
@@ -3538,18 +3538,18 @@
     </row>
     <row outlineLevel="0" r="168">
       <c r="A168" s="0">
-        <v>280</v>
+        <v>206</v>
       </c>
       <c r="B168" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect William Rehm</t>
+          <t>Bill Rehm Committee</t>
         </is>
       </c>
       <c r="C168" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D168" s="1">
-        <v>41995</v>
+        <v>41647.5109582986</v>
       </c>
       <c r="E168" s="0">
         <v>2</v>
@@ -3557,18 +3557,18 @@
     </row>
     <row outlineLevel="0" r="169">
       <c r="A169" s="0">
-        <v>281</v>
+        <v>207</v>
       </c>
       <c r="B169" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Dona Irwin</t>
+          <t>Susana Martinez Committee</t>
         </is>
       </c>
       <c r="C169" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D169" s="1">
-        <v>41995</v>
+        <v>41647.5116151273</v>
       </c>
       <c r="E169" s="0">
         <v>2</v>
@@ -3576,18 +3576,18 @@
     </row>
     <row outlineLevel="0" r="170">
       <c r="A170" s="0">
-        <v>282</v>
+        <v>208</v>
       </c>
       <c r="B170" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Andrew Nunez</t>
+          <t>Bobby Gonzales Committee</t>
         </is>
       </c>
       <c r="C170" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D170" s="1">
-        <v>41995</v>
+        <v>41647.5981723727</v>
       </c>
       <c r="E170" s="0">
         <v>2</v>
@@ -3595,18 +3595,18 @@
     </row>
     <row outlineLevel="0" r="171">
       <c r="A171" s="0">
-        <v>283</v>
+        <v>209</v>
       </c>
       <c r="B171" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Terry Mcmillan</t>
+          <t>Debbie Rodella Committee</t>
         </is>
       </c>
       <c r="C171" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D171" s="1">
-        <v>41995</v>
+        <v>41647.6055184838</v>
       </c>
       <c r="E171" s="0">
         <v>2</v>
@@ -3614,18 +3614,18 @@
     </row>
     <row outlineLevel="0" r="172">
       <c r="A172" s="0">
-        <v>284</v>
+        <v>210</v>
       </c>
       <c r="B172" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Diane Hamilton</t>
+          <t>Ken Martinez Committee</t>
         </is>
       </c>
       <c r="C172" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D172" s="1">
-        <v>41995</v>
+        <v>41647.6099128472</v>
       </c>
       <c r="E172" s="0">
         <v>2</v>
@@ -3633,18 +3633,18 @@
     </row>
     <row outlineLevel="0" r="173">
       <c r="A173" s="0">
-        <v>285</v>
+        <v>211</v>
       </c>
       <c r="B173" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Jane Powdrell-Culbert</t>
+          <t>Doreen Gallegos Committee</t>
         </is>
       </c>
       <c r="C173" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D173" s="1">
-        <v>41995</v>
+        <v>41647.613925081</v>
       </c>
       <c r="E173" s="0">
         <v>2</v>
@@ -3652,18 +3652,18 @@
     </row>
     <row outlineLevel="0" r="174">
       <c r="A174" s="0">
-        <v>286</v>
+        <v>212</v>
       </c>
       <c r="B174" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Carl Trujillo</t>
+          <t>Rick Miera Committee</t>
         </is>
       </c>
       <c r="C174" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D174" s="1">
-        <v>41995</v>
+        <v>41647.6175880787</v>
       </c>
       <c r="E174" s="0">
         <v>2</v>
@@ -3671,18 +3671,18 @@
     </row>
     <row outlineLevel="0" r="175">
       <c r="A175" s="0">
-        <v>287</v>
+        <v>213</v>
       </c>
       <c r="B175" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Don Tripp</t>
+          <t>Tom Taylor Commitee</t>
         </is>
       </c>
       <c r="C175" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D175" s="1">
-        <v>41995</v>
+        <v>41647.618943669</v>
       </c>
       <c r="E175" s="0">
         <v>2</v>
@@ -3690,18 +3690,18 @@
     </row>
     <row outlineLevel="0" r="176">
       <c r="A176" s="0">
-        <v>288</v>
+        <v>214</v>
       </c>
       <c r="B176" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Yvette Herrell</t>
+          <t>Rudy Martinez Committee</t>
         </is>
       </c>
       <c r="C176" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D176" s="1">
-        <v>41995</v>
+        <v>41647.6198285532</v>
       </c>
       <c r="E176" s="0">
         <v>2</v>
@@ -3709,18 +3709,18 @@
     </row>
     <row outlineLevel="0" r="177">
       <c r="A177" s="0">
-        <v>289</v>
+        <v>215</v>
       </c>
       <c r="B177" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Ricky Little</t>
+          <t>Bill Sharer Committee</t>
         </is>
       </c>
       <c r="C177" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D177" s="1">
-        <v>41995</v>
+        <v>41647.6209264699</v>
       </c>
       <c r="E177" s="0">
         <v>2</v>
@@ -3728,18 +3728,18 @@
     </row>
     <row outlineLevel="0" r="178">
       <c r="A178" s="0">
-        <v>290</v>
+        <v>216</v>
       </c>
       <c r="B178" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Cathrynn Brown</t>
+          <t>Hector Balderos Committee</t>
         </is>
       </c>
       <c r="C178" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D178" s="1">
-        <v>41995</v>
+        <v>41647.6218800579</v>
       </c>
       <c r="E178" s="0">
         <v>2</v>
@@ -3747,18 +3747,18 @@
     </row>
     <row outlineLevel="0" r="179">
       <c r="A179" s="0">
-        <v>291</v>
+        <v>217</v>
       </c>
       <c r="B179" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Jason Harper</t>
+          <t>Mary Kay Papen Committee</t>
         </is>
       </c>
       <c r="C179" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D179" s="1">
-        <v>41995</v>
+        <v>41647.6244457176</v>
       </c>
       <c r="E179" s="0">
         <v>2</v>
@@ -3766,18 +3766,18 @@
     </row>
     <row outlineLevel="0" r="180">
       <c r="A180" s="0">
-        <v>292</v>
+        <v>218</v>
       </c>
       <c r="B180" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Candy Ezzell</t>
+          <t>Michael Sanchez Committee</t>
         </is>
       </c>
       <c r="C180" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D180" s="1">
-        <v>41995</v>
+        <v>41647.6254394676</v>
       </c>
       <c r="E180" s="0">
         <v>2</v>
@@ -3785,18 +3785,18 @@
     </row>
     <row outlineLevel="0" r="181">
       <c r="A181" s="0">
-        <v>293</v>
+        <v>219</v>
       </c>
       <c r="B181" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Nora Espinoza</t>
+          <t>Steve Neville Committee</t>
         </is>
       </c>
       <c r="C181" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D181" s="1">
-        <v>41995</v>
+        <v>41647.6273356134</v>
       </c>
       <c r="E181" s="0">
         <v>2</v>
@@ -3804,18 +3804,18 @@
     </row>
     <row outlineLevel="0" r="182">
       <c r="A182" s="0">
-        <v>294</v>
+        <v>220</v>
       </c>
       <c r="B182" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Tim Lewis</t>
+          <t>Mark Moores Committee</t>
         </is>
       </c>
       <c r="C182" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D182" s="1">
-        <v>41995</v>
+        <v>41647.7168352199</v>
       </c>
       <c r="E182" s="0">
         <v>2</v>
@@ -3823,18 +3823,18 @@
     </row>
     <row outlineLevel="0" r="183">
       <c r="A183" s="0">
-        <v>295</v>
+        <v>221</v>
       </c>
       <c r="B183" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect David Gallegos</t>
+          <t>Christine Trujillo Committee</t>
         </is>
       </c>
       <c r="C183" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D183" s="1">
-        <v>41995</v>
+        <v>41647.7179861111</v>
       </c>
       <c r="E183" s="0">
         <v>2</v>
@@ -3842,18 +3842,18 @@
     </row>
     <row outlineLevel="0" r="184">
       <c r="A184" s="0">
-        <v>296</v>
+        <v>222</v>
       </c>
       <c r="B184" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Larry Scott</t>
+          <t>John Smith Committee</t>
         </is>
       </c>
       <c r="C184" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D184" s="1">
-        <v>41995</v>
+        <v>41647.7189679051</v>
       </c>
       <c r="E184" s="0">
         <v>2</v>
@@ -3861,18 +3861,18 @@
     </row>
     <row outlineLevel="0" r="185">
       <c r="A185" s="0">
-        <v>297</v>
+        <v>223</v>
       </c>
       <c r="B185" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect George Dodge</t>
+          <t>Michael Sanchez Committee</t>
         </is>
       </c>
       <c r="C185" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D185" s="1">
-        <v>41995</v>
+        <v>41647.720497338</v>
       </c>
       <c r="E185" s="0">
         <v>2</v>
@@ -3880,18 +3880,18 @@
     </row>
     <row outlineLevel="0" r="186">
       <c r="A186" s="0">
-        <v>298</v>
+        <v>224</v>
       </c>
       <c r="B186" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect James Madelena</t>
+          <t>Howie Morales Committee</t>
         </is>
       </c>
       <c r="C186" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D186" s="1">
-        <v>41995</v>
+        <v>41647.7212693634</v>
       </c>
       <c r="E186" s="0">
         <v>2</v>
@@ -3899,18 +3899,18 @@
     </row>
     <row outlineLevel="0" r="187">
       <c r="A187" s="0">
-        <v>299</v>
+        <v>225</v>
       </c>
       <c r="B187" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Bob Wooley</t>
+          <t>Sander Rue Committee</t>
         </is>
       </c>
       <c r="C187" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D187" s="1">
-        <v>41995</v>
+        <v>41647.7222477199</v>
       </c>
       <c r="E187" s="0">
         <v>2</v>
@@ -3918,18 +3918,18 @@
     </row>
     <row outlineLevel="0" r="188">
       <c r="A188" s="0">
-        <v>300</v>
+        <v>226</v>
       </c>
       <c r="B188" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Dennis Roch</t>
+          <t>Alonzo Baldonado Committee</t>
         </is>
       </c>
       <c r="C188" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D188" s="1">
-        <v>41995</v>
+        <v>41648.6875886227</v>
       </c>
       <c r="E188" s="0">
         <v>2</v>
@@ -3937,18 +3937,18 @@
     </row>
     <row outlineLevel="0" r="189">
       <c r="A189" s="0">
-        <v>301</v>
+        <v>227</v>
       </c>
       <c r="B189" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Monica Youngblood</t>
+          <t>Gail Chasey Committee</t>
         </is>
       </c>
       <c r="C189" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D189" s="1">
-        <v>41995</v>
+        <v>41648.6884904745</v>
       </c>
       <c r="E189" s="0">
         <v>2</v>
@@ -3956,18 +3956,18 @@
     </row>
     <row outlineLevel="0" r="190">
       <c r="A190" s="0">
-        <v>302</v>
+        <v>228</v>
       </c>
       <c r="B190" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Ken Martinez</t>
+          <t>Ernest Chavez Committee</t>
         </is>
       </c>
       <c r="C190" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D190" s="1">
-        <v>41995</v>
+        <v>41648.6893207523</v>
       </c>
       <c r="E190" s="0">
         <v>2</v>
@@ -3975,18 +3975,18 @@
     </row>
     <row outlineLevel="0" r="191">
       <c r="A191" s="0">
-        <v>303</v>
+        <v>229</v>
       </c>
       <c r="B191" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Vickie Perea</t>
+          <t>Sharon Clahchischilliage Committee</t>
         </is>
       </c>
       <c r="C191" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D191" s="1">
-        <v>41995</v>
+        <v>41648.6903244213</v>
       </c>
       <c r="E191" s="0">
         <v>2</v>
@@ -3994,18 +3994,18 @@
     </row>
     <row outlineLevel="0" r="192">
       <c r="A192" s="0">
-        <v>304</v>
+        <v>230</v>
       </c>
       <c r="B192" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Geoff Rodgers</t>
+          <t>Stephanie Garcia Richard Committee</t>
         </is>
       </c>
       <c r="C192" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D192" s="1">
-        <v>41995</v>
+        <v>41648.6926665509</v>
       </c>
       <c r="E192" s="0">
         <v>2</v>
@@ -4013,18 +4013,18 @@
     </row>
     <row outlineLevel="0" r="193">
       <c r="A193" s="0">
-        <v>305</v>
+        <v>231</v>
       </c>
       <c r="B193" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Betty Bishop</t>
+          <t>Jason Harper Committee</t>
         </is>
       </c>
       <c r="C193" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D193" s="1">
-        <v>41995</v>
+        <v>41648.6935905093</v>
       </c>
       <c r="E193" s="0">
         <v>2</v>
@@ -4032,18 +4032,18 @@
     </row>
     <row outlineLevel="0" r="194">
       <c r="A194" s="0">
-        <v>306</v>
+        <v>232</v>
       </c>
       <c r="B194" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Johnny Luevano</t>
+          <t>Georgene Louis Committee</t>
         </is>
       </c>
       <c r="C194" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D194" s="1">
-        <v>41995</v>
+        <v>41648.6945314468</v>
       </c>
       <c r="E194" s="0">
         <v>2</v>
@@ -4051,18 +4051,18 @@
     </row>
     <row outlineLevel="0" r="195">
       <c r="A195" s="0">
-        <v>307</v>
+        <v>233</v>
       </c>
       <c r="B195" s="0" t="inlineStr">
         <is>
-          <t>Committee to elect Sandra Jeff</t>
+          <t>James Smith Committee</t>
         </is>
       </c>
       <c r="C195" s="0">
-        <v>3012</v>
+        <v>2351</v>
       </c>
       <c r="D195" s="1">
-        <v>41995</v>
+        <v>41648.6987031597</v>
       </c>
       <c r="E195" s="0">
         <v>2</v>

</xml_diff>